<commit_message>
Ads implemented, icons added, basically ready to be shipped????????
</commit_message>
<xml_diff>
--- a/Non-Unity Files/Tap Tap Tilez - Achievement Details.xlsx
+++ b/Non-Unity Files/Tap Tap Tilez - Achievement Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a/Documents/GitHub/TileTapper/Non-Unity Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3FD225-E654-BC49-A9C0-2232015CC9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF2B1E4-05EE-5A4B-8A2D-7D3E96C37117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="9160" windowWidth="28040" windowHeight="16720" xr2:uid="{CB7210AE-F4B9-9A47-94DB-0F6957B14E51}"/>
+    <workbookView xWindow="12820" yWindow="1100" windowWidth="29400" windowHeight="16720" xr2:uid="{CB7210AE-F4B9-9A47-94DB-0F6957B14E51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1038,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20EAD7A9-5ECC-3E4F-AB25-342198E357FA}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2172,7 +2172,7 @@
         <v>75</v>
       </c>
       <c r="D49" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="E49" t="s">
         <v>198</v>

</xml_diff>